<commit_message>
5 Modifiy Time Register updated
</commit_message>
<xml_diff>
--- a/Requirements/Testing/Test Cases.xlsx
+++ b/Requirements/Testing/Test Cases.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caeta\Desktop\Documents\Proyectos\TimeAdministrator\TimeAdministrator\Requirements\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5E4713-9E1E-4A0E-AF7A-CB0FE71ACE96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C727092-BC4A-4D24-B47F-98E465C14CCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20910" windowHeight="13740" tabRatio="696" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20910" windowHeight="13740" tabRatio="696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="6. Register New Workspace" sheetId="7" r:id="rId1"/>
-    <sheet name="8. Filter Labels" sheetId="3" r:id="rId2"/>
-    <sheet name="9. Remove Label" sheetId="1" r:id="rId3"/>
-    <sheet name="10. Modify Label" sheetId="2" r:id="rId4"/>
-    <sheet name="11. Import Csv" sheetId="6" r:id="rId5"/>
-    <sheet name="Others" sheetId="5" r:id="rId6"/>
-    <sheet name="Flags" sheetId="8" r:id="rId7"/>
+    <sheet name="5. Modify Time Register" sheetId="9" r:id="rId1"/>
+    <sheet name="6. Register New Workspace" sheetId="7" r:id="rId2"/>
+    <sheet name="8. Filter Labels" sheetId="3" r:id="rId3"/>
+    <sheet name="9. Remove Label" sheetId="1" r:id="rId4"/>
+    <sheet name="10. Modify Label" sheetId="2" r:id="rId5"/>
+    <sheet name="11. Import Csv" sheetId="6" r:id="rId6"/>
+    <sheet name="Others" sheetId="5" r:id="rId7"/>
+    <sheet name="Flags" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="272">
   <si>
     <t>Id</t>
   </si>
@@ -832,6 +833,21 @@
   </si>
   <si>
     <t>Can't be imported csv with less than 5 fields. The missing field must to be added from excel or from noteblock</t>
+  </si>
+  <si>
+    <t>Deselect a record from the main table</t>
+  </si>
+  <si>
+    <t>2. Data loaded</t>
+  </si>
+  <si>
+    <t>1. Select a random record from the main table</t>
+  </si>
+  <si>
+    <t>2. Press "ESC" key</t>
+  </si>
+  <si>
+    <t>1. The selected item is unselected</t>
   </si>
 </sst>
 </file>
@@ -1417,6 +1433,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1441,20 +1463,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1755,11 +1771,163 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852666D3-C5BC-4636-A5FB-DEAAE88879F7}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33" customWidth="1"/>
+    <col min="8" max="10" width="32.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="13" width="32.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="80" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="128" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="128" t="s">
+        <v>202</v>
+      </c>
+      <c r="F2" s="128" t="s">
+        <v>269</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="129"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36" t="s">
+        <v>268</v>
+      </c>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BB98C2-E7C8-4825-9740-CAB10EFBA8C5}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,7 +2343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{188C4133-60F2-43BD-8422-230B8F1707EF}">
   <dimension ref="A1:L119"/>
   <sheetViews>
@@ -4156,7 +4324,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M31"/>
   <sheetViews>
@@ -4752,7 +4920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8614EB4E-DBD6-4335-8AC7-592BA2F011D7}">
   <dimension ref="A1:N89"/>
   <sheetViews>
@@ -4825,28 +4993,28 @@
       <c r="A2" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="149" t="s">
+      <c r="B2" s="151" t="s">
         <v>140</v>
       </c>
       <c r="C2" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="149" t="s">
+      <c r="D2" s="151" t="s">
         <v>141</v>
       </c>
       <c r="E2" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="149" t="s">
+      <c r="F2" s="151" t="s">
         <v>137</v>
       </c>
-      <c r="G2" s="152" t="s">
+      <c r="G2" s="154" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="149" t="s">
+      <c r="H2" s="151" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="149" t="s">
+      <c r="I2" s="151" t="s">
         <v>145</v>
       </c>
       <c r="J2" s="57" t="s">
@@ -4855,7 +5023,7 @@
       <c r="K2" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="L2" s="149"/>
+      <c r="L2" s="151"/>
       <c r="M2" s="145" t="s">
         <v>145</v>
       </c>
@@ -4863,19 +5031,19 @@
     </row>
     <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="58"/>
-      <c r="B3" s="150"/>
+      <c r="B3" s="152"/>
       <c r="C3" s="59"/>
-      <c r="D3" s="150"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="60"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="153"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="150"/>
-      <c r="J3" s="150" t="s">
+      <c r="F3" s="152"/>
+      <c r="G3" s="155"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
+      <c r="J3" s="152" t="s">
         <v>143</v>
       </c>
       <c r="K3" s="61"/>
-      <c r="L3" s="150"/>
+      <c r="L3" s="152"/>
       <c r="M3" s="146"/>
       <c r="N3" s="61"/>
     </row>
@@ -4883,7 +5051,7 @@
       <c r="A4" s="58"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
-      <c r="D4" s="150" t="s">
+      <c r="D4" s="152" t="s">
         <v>37</v>
       </c>
       <c r="E4" s="60"/>
@@ -4893,9 +5061,9 @@
       <c r="G4" s="146" t="s">
         <v>136</v>
       </c>
-      <c r="H4" s="150"/>
+      <c r="H4" s="152"/>
       <c r="I4" s="59"/>
-      <c r="J4" s="150"/>
+      <c r="J4" s="152"/>
       <c r="K4" s="61"/>
       <c r="L4" s="63"/>
       <c r="M4" s="61"/>
@@ -4905,7 +5073,7 @@
       <c r="A5" s="58"/>
       <c r="B5" s="59"/>
       <c r="C5" s="59"/>
-      <c r="D5" s="150"/>
+      <c r="D5" s="152"/>
       <c r="E5" s="60"/>
       <c r="F5" s="62" t="s">
         <v>146</v>
@@ -4927,7 +5095,7 @@
       <c r="A6" s="58"/>
       <c r="B6" s="59"/>
       <c r="C6" s="60"/>
-      <c r="D6" s="150"/>
+      <c r="D6" s="152"/>
       <c r="E6" s="60"/>
       <c r="F6" s="59" t="s">
         <v>147</v>
@@ -4945,7 +5113,7 @@
       <c r="A7" s="58"/>
       <c r="B7" s="59"/>
       <c r="C7" s="60"/>
-      <c r="D7" s="150"/>
+      <c r="D7" s="152"/>
       <c r="E7" s="60"/>
       <c r="F7" s="59" t="s">
         <v>148</v>
@@ -4963,11 +5131,11 @@
       <c r="A8" s="58"/>
       <c r="B8" s="59"/>
       <c r="C8" s="60"/>
-      <c r="D8" s="150"/>
+      <c r="D8" s="152"/>
       <c r="E8" s="60"/>
       <c r="F8" s="65"/>
       <c r="G8" s="60"/>
-      <c r="H8" s="154"/>
+      <c r="H8" s="156"/>
       <c r="I8" s="65"/>
       <c r="J8" s="60"/>
       <c r="K8" s="61"/>
@@ -4994,7 +5162,7 @@
       <c r="F9" s="126" t="s">
         <v>149</v>
       </c>
-      <c r="G9" s="155" t="s">
+      <c r="G9" s="157" t="s">
         <v>132</v>
       </c>
       <c r="H9" s="66" t="s">
@@ -5020,7 +5188,7 @@
       <c r="D10" s="127"/>
       <c r="E10" s="71"/>
       <c r="F10" s="127"/>
-      <c r="G10" s="156"/>
+      <c r="G10" s="158"/>
       <c r="H10" s="67" t="s">
         <v>123</v>
       </c>
@@ -5042,7 +5210,7 @@
       <c r="F11" s="67" t="s">
         <v>150</v>
       </c>
-      <c r="G11" s="156" t="s">
+      <c r="G11" s="158" t="s">
         <v>136</v>
       </c>
       <c r="H11" s="67" t="s">
@@ -5070,12 +5238,12 @@
       <c r="F12" s="67" t="s">
         <v>146</v>
       </c>
-      <c r="G12" s="156"/>
+      <c r="G12" s="158"/>
       <c r="H12" s="127" t="s">
         <v>133</v>
       </c>
       <c r="I12" s="67"/>
-      <c r="J12" s="157" t="s">
+      <c r="J12" s="161" t="s">
         <v>133</v>
       </c>
       <c r="K12" s="71"/>
@@ -5095,7 +5263,7 @@
       <c r="G13" s="72"/>
       <c r="H13" s="127"/>
       <c r="I13" s="67"/>
-      <c r="J13" s="157"/>
+      <c r="J13" s="161"/>
       <c r="K13" s="71"/>
       <c r="L13" s="36"/>
       <c r="M13" s="36"/>
@@ -5115,7 +5283,7 @@
       <c r="G14" s="72"/>
       <c r="H14" s="127"/>
       <c r="I14" s="67"/>
-      <c r="J14" s="157"/>
+      <c r="J14" s="161"/>
       <c r="K14" s="71"/>
       <c r="L14" s="36"/>
       <c r="M14" s="36"/>
@@ -5149,7 +5317,7 @@
       <c r="C16" s="91" t="s">
         <v>163</v>
       </c>
-      <c r="D16" s="149" t="s">
+      <c r="D16" s="151" t="s">
         <v>182</v>
       </c>
       <c r="E16" s="92" t="s">
@@ -5181,10 +5349,10 @@
       <c r="A17" s="79"/>
       <c r="B17" s="146"/>
       <c r="C17" s="61"/>
-      <c r="D17" s="150"/>
+      <c r="D17" s="152"/>
       <c r="E17" s="60"/>
       <c r="F17" s="163"/>
-      <c r="G17" s="150" t="s">
+      <c r="G17" s="152" t="s">
         <v>136</v>
       </c>
       <c r="H17" s="78" t="s">
@@ -5210,7 +5378,7 @@
       <c r="F18" s="94" t="s">
         <v>174</v>
       </c>
-      <c r="G18" s="150"/>
+      <c r="G18" s="152"/>
       <c r="H18" s="78" t="s">
         <v>124</v>
       </c>
@@ -5309,7 +5477,7 @@
       <c r="E23" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="158" t="s">
+      <c r="F23" s="159" t="s">
         <v>149</v>
       </c>
       <c r="G23" s="128" t="s">
@@ -5333,7 +5501,7 @@
       <c r="C24" s="36"/>
       <c r="D24" s="127"/>
       <c r="E24" s="107"/>
-      <c r="F24" s="159"/>
+      <c r="F24" s="160"/>
       <c r="G24" s="129"/>
       <c r="H24" s="85" t="s">
         <v>123</v>
@@ -5409,7 +5577,7 @@
       <c r="A28" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="B28" s="160" t="s">
+      <c r="B28" s="149" t="s">
         <v>49</v>
       </c>
       <c r="C28" s="32" t="s">
@@ -5424,7 +5592,7 @@
       <c r="F28" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="G28" s="160" t="s">
+      <c r="G28" s="149" t="s">
         <v>197</v>
       </c>
       <c r="H28" s="84" t="s">
@@ -5439,14 +5607,14 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="87"/>
-      <c r="B29" s="161"/>
+      <c r="B29" s="150"/>
       <c r="C29" s="36"/>
       <c r="D29" s="127"/>
       <c r="E29" s="40"/>
       <c r="F29" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="G29" s="161"/>
+      <c r="G29" s="150"/>
       <c r="H29" s="85" t="s">
         <v>123</v>
       </c>
@@ -5705,7 +5873,7 @@
       <c r="C41" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="149" t="s">
+      <c r="D41" s="151" t="s">
         <v>101</v>
       </c>
       <c r="E41" s="92" t="s">
@@ -5717,7 +5885,7 @@
       <c r="G41" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="H41" s="149" t="s">
+      <c r="H41" s="151" t="s">
         <v>33</v>
       </c>
       <c r="I41" s="91"/>
@@ -5733,13 +5901,13 @@
       <c r="A42" s="102"/>
       <c r="B42" s="165"/>
       <c r="C42" s="61"/>
-      <c r="D42" s="150"/>
+      <c r="D42" s="152"/>
       <c r="E42" s="60"/>
       <c r="F42" s="95" t="s">
         <v>11</v>
       </c>
       <c r="G42" s="61"/>
-      <c r="H42" s="150"/>
+      <c r="H42" s="152"/>
       <c r="I42" s="61"/>
       <c r="J42" s="63"/>
       <c r="K42" s="63"/>
@@ -5751,13 +5919,13 @@
       <c r="A43" s="102"/>
       <c r="B43" s="165"/>
       <c r="C43" s="61"/>
-      <c r="D43" s="150"/>
+      <c r="D43" s="152"/>
       <c r="E43" s="60"/>
       <c r="F43" s="95" t="s">
         <v>12</v>
       </c>
       <c r="G43" s="61"/>
-      <c r="H43" s="150"/>
+      <c r="H43" s="152"/>
       <c r="I43" s="61"/>
       <c r="J43" s="63"/>
       <c r="K43" s="63"/>
@@ -6102,7 +6270,7 @@
       <c r="F60" s="126" t="s">
         <v>149</v>
       </c>
-      <c r="G60" s="155" t="s">
+      <c r="G60" s="157" t="s">
         <v>132</v>
       </c>
       <c r="H60" s="97" t="s">
@@ -6126,7 +6294,7 @@
       <c r="D61" s="129"/>
       <c r="E61" s="129"/>
       <c r="F61" s="127"/>
-      <c r="G61" s="156"/>
+      <c r="G61" s="158"/>
       <c r="H61" s="98" t="s">
         <v>123</v>
       </c>
@@ -6150,7 +6318,7 @@
       <c r="F62" s="98" t="s">
         <v>208</v>
       </c>
-      <c r="G62" s="156" t="s">
+      <c r="G62" s="158" t="s">
         <v>136</v>
       </c>
       <c r="H62" s="98" t="s">
@@ -6174,7 +6342,7 @@
       <c r="F63" s="98" t="s">
         <v>146</v>
       </c>
-      <c r="G63" s="156"/>
+      <c r="G63" s="158"/>
       <c r="H63" s="127" t="s">
         <v>198</v>
       </c>
@@ -6215,9 +6383,9 @@
         <v>148</v>
       </c>
       <c r="G65" s="43"/>
-      <c r="H65" s="151"/>
+      <c r="H65" s="153"/>
       <c r="I65" s="41"/>
-      <c r="J65" s="151"/>
+      <c r="J65" s="153"/>
       <c r="K65" s="41"/>
       <c r="L65" s="42"/>
       <c r="M65" s="41"/>
@@ -6883,11 +7051,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05760916-9E37-49D1-B48B-D94D47CC4A32}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
@@ -6979,7 +7147,7 @@
       </c>
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
-      <c r="L2" s="160"/>
+      <c r="L2" s="149"/>
       <c r="M2" s="32"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -7000,7 +7168,7 @@
       </c>
       <c r="J3" s="36"/>
       <c r="K3" s="36"/>
-      <c r="L3" s="161"/>
+      <c r="L3" s="150"/>
       <c r="M3" s="36"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -8051,7 +8219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B04E03A-7463-4C8E-ADAF-9D8D097F56C8}">
   <dimension ref="A1:L23"/>
   <sheetViews>
@@ -8516,7 +8684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A698848C-6CA0-46C2-AD66-73B70DBE28FC}">
   <dimension ref="A1:B5"/>
   <sheetViews>

</xml_diff>